<commit_message>
get rid of "geo" epivar in favor of lat/lon
I realized that this epivar made no sense since it made everything
a bit more complex than it needed to be. I'm replacing it with
geo_lon and geo_lat. The geo() accessor will still exist to return
the lon and lat columns in the correct plotting order.
</commit_message>
<xml_diff>
--- a/inst/example_dict.xlsx
+++ b/inst/example_dict.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t xml:space="preserve">epivar</t>
   </si>
@@ -98,22 +98,13 @@
     <t xml:space="preserve">age group of the individual in years</t>
   </si>
   <si>
-    <t xml:space="preserve">geo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#geo +lon +lat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">geographic coordinate: longitude, latitude</t>
-  </si>
-  <si>
     <t xml:space="preserve">geo_lon</t>
   </si>
   <si>
     <t xml:space="preserve">#geo +lon</t>
   </si>
   <si>
-    <t xml:space="preserve">longitude in degrees</t>
+    <t xml:space="preserve">geographic coordinate: longitude</t>
   </si>
   <si>
     <t xml:space="preserve">geo_lat</t>
@@ -122,7 +113,7 @@
     <t xml:space="preserve">#geo +lat</t>
   </si>
   <si>
-    <t xml:space="preserve">latitude in degrees</t>
+    <t xml:space="preserve">geographic coordinate: latitude</t>
   </si>
 </sst>
 </file>
@@ -586,17 +577,6 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" t="s">
-        <v>36</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>